<commit_message>
Used 55.2 VDC instead of 55.6 VDC for absorbption voltage. Everything is ran in open-loop so better to keep it a little bit low (3.45 VDC / cell)
</commit_message>
<xml_diff>
--- a/strategy/2024-01-13.xlsx
+++ b/strategy/2024-01-13.xlsx
@@ -312,7 +312,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F28" activeCellId="0" sqref="F28"/>
+      <selection pane="topLeft" activeCell="H25" activeCellId="0" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -385,7 +385,7 @@
         <v>192</v>
       </c>
       <c r="G3" s="1" t="n">
-        <v>55.6</v>
+        <v>55.2</v>
       </c>
       <c r="H3" s="7" t="n">
         <v>50</v>
@@ -414,7 +414,7 @@
         <v>194</v>
       </c>
       <c r="G4" s="1" t="n">
-        <v>55.6</v>
+        <v>55.2</v>
       </c>
       <c r="H4" s="1" t="n">
         <f aca="false">$H$3</f>
@@ -444,7 +444,7 @@
         <v>193</v>
       </c>
       <c r="G5" s="1" t="n">
-        <v>55.6</v>
+        <v>55.2</v>
       </c>
       <c r="H5" s="1" t="n">
         <f aca="false">$H$3</f>
@@ -474,7 +474,7 @@
         <v>191</v>
       </c>
       <c r="G6" s="1" t="n">
-        <v>55.6</v>
+        <v>55.2</v>
       </c>
       <c r="H6" s="1" t="n">
         <f aca="false">$H$3</f>
@@ -504,7 +504,7 @@
         <v>192</v>
       </c>
       <c r="G7" s="1" t="n">
-        <v>55.6</v>
+        <v>55.2</v>
       </c>
       <c r="H7" s="1" t="n">
         <f aca="false">$H$3</f>
@@ -534,7 +534,7 @@
         <v>188</v>
       </c>
       <c r="G8" s="1" t="n">
-        <v>55.6</v>
+        <v>55.2</v>
       </c>
       <c r="H8" s="1" t="n">
         <f aca="false">$H$3</f>
@@ -564,7 +564,7 @@
         <v>213</v>
       </c>
       <c r="G9" s="1" t="n">
-        <v>55.6</v>
+        <v>55.2</v>
       </c>
       <c r="H9" s="1" t="n">
         <f aca="false">$H$3</f>
@@ -594,7 +594,7 @@
         <v>216</v>
       </c>
       <c r="G10" s="1" t="n">
-        <v>55.6</v>
+        <v>55.2</v>
       </c>
       <c r="H10" s="1" t="n">
         <f aca="false">$H$3</f>
@@ -624,7 +624,7 @@
         <v>215</v>
       </c>
       <c r="G11" s="1" t="n">
-        <v>55.6</v>
+        <v>55.2</v>
       </c>
       <c r="H11" s="1" t="n">
         <f aca="false">$H$3</f>
@@ -654,7 +654,7 @@
         <v>220</v>
       </c>
       <c r="G12" s="1" t="n">
-        <v>55.6</v>
+        <v>55.2</v>
       </c>
       <c r="H12" s="1" t="n">
         <f aca="false">$H$3</f>
@@ -684,7 +684,7 @@
         <v>219</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>55.6</v>
+        <v>55.2</v>
       </c>
       <c r="H13" s="1" t="n">
         <f aca="false">$H$3</f>
@@ -714,7 +714,7 @@
         <v>218</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>55.6</v>
+        <v>55.2</v>
       </c>
       <c r="H14" s="1" t="n">
         <f aca="false">$H$3</f>
@@ -744,7 +744,7 @@
         <v>217</v>
       </c>
       <c r="G15" s="1" t="n">
-        <v>55.6</v>
+        <v>55.2</v>
       </c>
       <c r="H15" s="1" t="n">
         <f aca="false">$H$3</f>
@@ -774,7 +774,7 @@
         <v>211</v>
       </c>
       <c r="G16" s="1" t="n">
-        <v>55.6</v>
+        <v>55.2</v>
       </c>
       <c r="H16" s="1" t="n">
         <f aca="false">$H$3</f>
@@ -804,7 +804,7 @@
         <v>215</v>
       </c>
       <c r="G17" s="1" t="n">
-        <v>55.6</v>
+        <v>55.2</v>
       </c>
       <c r="H17" s="1" t="n">
         <f aca="false">$H$3</f>
@@ -834,7 +834,7 @@
         <v>216</v>
       </c>
       <c r="G18" s="1" t="n">
-        <v>55.6</v>
+        <v>55.2</v>
       </c>
       <c r="H18" s="1" t="n">
         <f aca="false">$H$3</f>
@@ -864,7 +864,7 @@
         <v>218</v>
       </c>
       <c r="G19" s="1" t="n">
-        <v>55.6</v>
+        <v>55.2</v>
       </c>
       <c r="H19" s="1" t="n">
         <f aca="false">$H$3</f>
@@ -1014,7 +1014,7 @@
         <v>218</v>
       </c>
       <c r="G24" s="1" t="n">
-        <v>55.6</v>
+        <v>55.2</v>
       </c>
       <c r="H24" s="1" t="n">
         <f aca="false">$H$3</f>
@@ -1044,7 +1044,7 @@
         <v>212</v>
       </c>
       <c r="G25" s="1" t="n">
-        <v>55.6</v>
+        <v>55.2</v>
       </c>
       <c r="H25" s="1" t="n">
         <f aca="false">$H$3</f>
@@ -1074,7 +1074,7 @@
         <v>211</v>
       </c>
       <c r="G26" s="1" t="n">
-        <v>55.6</v>
+        <v>55.2</v>
       </c>
       <c r="H26" s="1" t="n">
         <f aca="false">$H$3</f>

</xml_diff>